<commit_message>
Modified event generation test cases for HPA Notification
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
+++ b/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Event Generation" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="130">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -158,24 +158,12 @@
     <t>X-1P-User=(SYS_USER1)</t>
   </si>
   <si>
-    <t>OPQA-3993</t>
-  </si>
-  <si>
-    <t>Verify that user is able to create a new Watchlist using container API</t>
-  </si>
-  <si>
     <t>/container</t>
   </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>{ "name": "Watchlist for HPA BatchJob", "desc": "","type": "watchlist" }</t>
-  </si>
-  <si>
-    <t>status=200||userid=(SYS_USER1)||ispublic=false</t>
-  </si>
-  <si>
     <t>/container/(OPQA-3993_id)</t>
   </si>
   <si>
@@ -215,48 +203,9 @@
     <t>/patents/search</t>
   </si>
   <si>
-    <t>OPQA-xxxx1</t>
-  </si>
-  <si>
-    <t>Verify that user is able to add comment on a patent</t>
-  </si>
-  <si>
     <t>x-1p-user=(SYS_USER3)||Content-Type=application/json</t>
   </si>
   <si>
-    <t>status=200||comments.userId=(SYS_USER3)</t>
-  </si>
-  <si>
-    <t>OPQA-xxxx2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that user is able to appreciate the comments of patent </t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/Comment/(OPQA-xxxx1_comments.id)</t>
-  </si>
-  <si>
-    <t>x-1p-user=(SYS_USER1)||Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-xxxx1_comments.id)</t>
-  </si>
-  <si>
-    <t>OPQA-xxxx6</t>
-  </si>
-  <si>
-    <t>Verify that user able to delete comment</t>
-  </si>
-  <si>
-    <t>OPQA-286</t>
-  </si>
-  <si>
-    <t>/comments/comment/(OPQA-xxxx6_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-xxxx6_comments.id)</t>
-  </si>
-  <si>
     <t>OPQA-3951</t>
   </si>
   <si>
@@ -266,9 +215,6 @@
     <t>X-1P-User=(SYS_USER3)</t>
   </si>
   <si>
-    <t>Verify that user is able to get comments of patent by passing patent id</t>
-  </si>
-  <si>
     <t>OPQA-898_1</t>
   </si>
   <si>
@@ -281,22 +227,10 @@
     <t>hits.hits._id[1]</t>
   </si>
   <si>
-    <t>/comments/(OPQA-898_hits.hits._id[1])/patents</t>
-  </si>
-  <si>
-    <t>{"targetType":"patents","targetId":"(OPQA-898_1_hits.hits._id[1])","content":"Notification Test"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.targetType=patents||comments.targetId=(OPQA-898_hits.hits._id[1])</t>
-  </si>
-  <si>
     <t>private.desc</t>
   </si>
   <si>
     <t>OPQA-312</t>
-  </si>
-  <si>
-    <t>Verify that user able to create public watchlist</t>
   </si>
   <si>
     <t>/container/</t>
@@ -365,9 +299,6 @@
     <t>Verify that user receives a notification when someone he is following comments on an article</t>
   </si>
   <si>
-    <t>{ "desc": "id[0]:(OPQA-236_comments.id):: id[1]:(OPQA-xxxx1_comments.id)::id[2]:(OPQA-874_hits.hits._id)::id[3]:(OPQA-898_hits.hits._id[1])"}</t>
-  </si>
-  <si>
     <t>Verify that user can delete the comments user authored themselves and validate the comment count</t>
   </si>
   <si>
@@ -416,10 +347,76 @@
     <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-4135_id2)</t>
   </si>
   <si>
-    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-4135_id3)</t>
-  </si>
-  <si>
     <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-4135_id2)</t>
+  </si>
+  <si>
+    <t>OPQA-461</t>
+  </si>
+  <si>
+    <t>verify that user able to unfollow a following user</t>
+  </si>
+  <si>
+    <t>1PFOLLOW</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/following/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||followRelationship=IS_NONE</t>
+  </si>
+  <si>
+    <t>hits.hits._id[0]||hits.hits._id[1]</t>
+  </si>
+  <si>
+    <t>OPQA-450</t>
+  </si>
+  <si>
+    <t>Verify that Start following a user and verify the follow relationship for notification test.</t>
+  </si>
+  <si>
+    <t>status=201||followRelationship=IS_FOLLOWER</t>
+  </si>
+  <si>
+    <t>OPQA-1431</t>
+  </si>
+  <si>
+    <t>Verify that user2 create comment in user3 watching patent</t>
+  </si>
+  <si>
+    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.hits._id[1])","content":"Notification Test"}</t>
+  </si>
+  <si>
+    <t>OPQA-284_2</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Comment/(OPQA-1431_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-1431_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-284_3</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=2||targetId=(OPQA-1431_comments.id)</t>
+  </si>
+  <si>
+    <t>{ "desc": "id[0]:(OPQA-236_comments.id):: id[1]:(OPQA-1431_comments.id)::id[2]:(OPQA-874_hits.hits._id)::id[3]:(OPQA-898_hits.hits._id[0])::id[4]:(OPQA-898_hits.hits._id[1])"}</t>
+  </si>
+  <si>
+    <t>OPQA-1433</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following comments on a patent</t>
+  </si>
+  <si>
+    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-4135_id4)</t>
+  </si>
+  <si>
+    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-4135_id4)</t>
+  </si>
+  <si>
+    <t>Verify that user able to create watchlist</t>
   </si>
 </sst>
 </file>
@@ -846,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="G17" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -915,7 +912,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>14</v>
@@ -924,7 +921,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="6"/>
@@ -932,25 +929,25 @@
         <v>38</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>46</v>
@@ -966,199 +963,190 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
-      <c r="A5" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45">
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" s="9" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>30</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1" ht="45">
+      <c r="A7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="J8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="47.25">
+      <c r="A9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="5" customFormat="1">
-      <c r="A7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7"/>
-      <c r="G7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7"/>
-      <c r="J7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12" ht="30">
-      <c r="A8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" ht="47.25">
-      <c r="A10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="J10" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="9" t="s">
@@ -1255,23 +1243,23 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="6" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
@@ -1279,15 +1267,15 @@
         <v>38</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
       <c r="A15" s="9" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1295,178 +1283,177 @@
       <c r="D15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="5"/>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="9"/>
       <c r="H15" s="6" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
-      <c r="A16" s="9" t="s">
-        <v>70</v>
+      <c r="A16" t="s">
+        <v>119</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
         <v>20</v>
       </c>
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="5"/>
+      <c r="F16" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="H16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="60">
-      <c r="A17" s="3" t="s">
-        <v>92</v>
+        <v>116</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" t="s">
+        <v>122</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="105">
+      <c r="H17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" ht="60">
       <c r="A18" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>99</v>
+      <c r="D18" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" t="s">
-        <v>101</v>
-      </c>
+      <c r="F18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="5"/>
       <c r="J18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>50</v>
+        <v>74</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="105">
       <c r="A19" s="3" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>42</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="30">
-      <c r="A20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="105">
+      <c r="A20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="D20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60">
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75">
       <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
@@ -1477,7 +1464,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>43</v>
@@ -1486,7 +1473,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
@@ -1502,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1514,7 +1501,7 @@
     <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="32.5703125" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.7109375" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="93.28515625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="21" customWidth="1" collapsed="1"/>
@@ -1560,16 +1547,16 @@
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" ht="45">
       <c r="A2" s="6" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>14</v>
@@ -1578,7 +1565,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="6"/>
@@ -1586,7 +1573,7 @@
         <v>38</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="L2"/>
     </row>
@@ -1598,10 +1585,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -1610,115 +1597,115 @@
         <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="9" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" s="9" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="9" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="9" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -1727,42 +1714,42 @@
         <v>46</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="9" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified validations and logic for Decorator API
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
+++ b/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Event Generation" sheetId="1" r:id="rId1"/>
     <sheet name="Notification Test" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="147">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -404,22 +405,82 @@
     <t>{"queryRef":"notifyQrRef_V2","params":{"size":["20"],"byscore":["true"]}}</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-874_hits.hits._id)","content":"Notification Test (ddMMMyyyy_HHmmss)"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.hits._id[1])","content":"Notification Test (ddMMMyyyy_HHmmss)"}</t>
-  </si>
-  <si>
     <t>comments.id||comments.content</t>
   </si>
   <si>
-    <t>{ "desc": "id[0]:(OPQA-236_comments.id):: id[1]:(OPQA-1431_comments.id)::id[2]:(OPQA-874_hits.hits._id)::id[3]:(OPQA-898_hits.hits._id[0])::id[4]:(OPQA-898_hits.hits._id[1])::id[5]:(OPQA-236_comments.content)::id[6]:(OPQA-1431_comments.content)"}</t>
-  </si>
-  <si>
     <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER2)||notify.comments.content=(OPQA-4135_id5)||notify.document.id=(OPQA-4135_id2)||notify.document.type=wos</t>
   </si>
   <si>
     <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER2)||notify.comments.content=(OPQA-4135_id6)||notify.document.id=(OPQA-4135_id4)||notify.document.type=patents</t>
+  </si>
+  <si>
+    <t>notify.pitoId[19]</t>
+  </si>
+  <si>
+    <t>{ "desc": "id[0]:(OPQA-236_comments.id), id[1]:(OPQA-1431_comments.id),id[2]:(OPQA-874_hits.hits._id),id[3]:(OPQA-898_hits.hits._id[0]),id[4]:(OPQA-898_hits.hits._id[1]),id[5]:(OPQA-236_comments.content),id[6]:(OPQA-1431_comments.content)"}</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=DocumentComment||notify.issuerProfile.truid=(SYS_USER2)||notify.document.id=(OPQA-4135_id4)||notify.document.type=patents||notify.comments.id=(OPQA-4135_id1)||notify.comments.content=(OPQA-4135_id6)</t>
+  </si>
+  <si>
+    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.hits._id[1])","content":"Patents Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=DocumentComment||notify.issuerProfile.truid=(SYS_USER2)||notify.document.id=(OPQA-4135_id2)||notify.document.type=wos||notify.comments.id=(OPQA-4135_id0)||notify.comments.content=(OPQA-4135_id5)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-874_hits.hits._id)","content":"Article Notification Test (ddMMMyyyy_HHmmss) for HPA notify"}</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER1)||notify.issuer=(SYS_USER3)||notify.targetId=(OPQA-4135_id1)||notify.publicationRef.comment.content=(OPQA-4135_id6)||notify.publicationRef.comment.targetType=patents||notify.publicationRef.comment.publication.id=(OPQA-4135_id4)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER1)||notify.issuer=(SYS_USER3)||notify.comments.targetId=(OPQA-4135_id0)||notify.publicationRef.comment.content=(OPQA-4135_id5)||notify.publicationRef.comment.targetType=wos||notify.publicationRef.comment.publication.id=(OPQA-4135_id2)</t>
+  </si>
+  <si>
+    <t>1PSEARCHV4</t>
+  </si>
+  <si>
+    <t>hits.id</t>
+  </si>
+  <si>
+    <t>hits.id[0]||hits.id[1]</t>
+  </si>
+  <si>
+    <t>hits.id[1]</t>
+  </si>
+  <si>
+    <t>/comments/(OPQA-874_hits.id)/wos</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-874_hits.id)||id=(OPQA-253_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-874_hits.id)","content":"Article Notification Test (ddMMMyyyy_HHmmss) for HPA Batch job"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.id[1])","content":"Patents Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>{
+"items":
+[{
+"id":"(OPQA-874_hits.id)",
+"type":"wos"
+}]
+}</t>
+  </si>
+  <si>
+    <t>{
+"items":
+[{
+"id":"(OPQA-898_hits.id[1])",
+"type":"patents"
+}]
+}</t>
+  </si>
+  <si>
+    <t>{ "desc": "id[0]:(OPQA-236_comments.id), id[1]:(OPQA-1431_comments.id),id[2]:(OPQA-874_hits.id),id[3]:(OPQA-898_hits.id[0]),id[4]:(OPQA-898_hits.id[1]),id[5]:(OPQA-236_comments.content),id[6]:(OPQA-1431_comments.content)"}</t>
   </si>
 </sst>
 </file>
@@ -846,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="G16" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
+      <selection activeCell="L22" sqref="L2:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -992,7 +1053,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>36</v>
@@ -1010,7 +1071,7 @@
         <v>37</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
@@ -1024,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>14</v>
@@ -1067,12 +1128,12 @@
         <v>91</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="30">
+    <row r="8" spans="1:12">
       <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
@@ -1080,7 +1141,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>60</v>
@@ -1096,7 +1157,7 @@
         <v>37</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="47.25">
@@ -1151,310 +1212,310 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="45">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:12" ht="60">
+      <c r="A11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="105">
+      <c r="A12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" ht="45">
+      <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="30">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45">
-      <c r="A15" s="9" t="s">
-        <v>110</v>
+      <c r="J14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" t="s">
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="105">
+      <c r="A17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45">
+      <c r="A18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="E18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I18" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30">
-      <c r="A16" t="s">
+      <c r="K18" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J19" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="30">
-      <c r="A17" t="s">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J20" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" ht="60">
-      <c r="A18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="105">
-      <c r="A19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="105">
-      <c r="A20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I20" t="s">
-        <v>83</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" s="6" t="s">
@@ -1505,7 +1566,7 @@
         <v>21</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
@@ -1521,7 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L8"/>
     </sheetView>
   </sheetViews>
@@ -1609,7 +1670,7 @@
       </c>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:12" ht="75">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1635,10 +1696,13 @@
         <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30">
+        <v>135</v>
+      </c>
+      <c r="K3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -1655,7 +1719,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>124</v>
@@ -1664,9 +1728,11 @@
         <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="6"/>
+        <v>134</v>
+      </c>
+      <c r="K4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" s="9" t="s">
@@ -1694,7 +1760,10 @@
         <v>100</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="K5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
@@ -1723,7 +1792,10 @@
         <v>100</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="K6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
@@ -1752,7 +1824,10 @@
         <v>100</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>37</v>
+        <v>132</v>
+      </c>
+      <c r="K7" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
@@ -1781,6 +1856,679 @@
         <v>100</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="44.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="J8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
+      <c r="A9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" ht="45">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="45">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="45">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" ht="60">
+      <c r="A18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="105">
+      <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="105">
+      <c r="A20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="105">
+      <c r="A22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Recommit the changes of Decorator API test cases validations.
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
+++ b/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Event Generation" sheetId="1" r:id="rId1"/>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1588,7 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Forgot API test cases in IAMTestData excel.
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
+++ b/src/test/test-data/DecoratorBatchJobTest_HPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="151">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -402,9 +402,6 @@
     <t>status=200||userid=(SYS_USER1)||ispublic=false</t>
   </si>
   <si>
-    <t>{"queryRef":"notifyQrRef_V2","params":{"size":["20"],"byscore":["true"]}}</t>
-  </si>
-  <si>
     <t>comments.id||comments.content</t>
   </si>
   <si>
@@ -430,12 +427,6 @@
   </si>
   <si>
     <t>{"targetType":"wos","targetId":"(OPQA-874_hits.hits._id)","content":"Article Notification Test (ddMMMyyyy_HHmmss) for HPA notify"}</t>
-  </si>
-  <si>
-    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER1)||notify.issuer=(SYS_USER3)||notify.targetId=(OPQA-4135_id1)||notify.publicationRef.comment.content=(OPQA-4135_id6)||notify.publicationRef.comment.targetType=patents||notify.publicationRef.comment.publication.id=(OPQA-4135_id4)</t>
-  </si>
-  <si>
-    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER1)||notify.issuer=(SYS_USER3)||notify.comments.targetId=(OPQA-4135_id0)||notify.publicationRef.comment.content=(OPQA-4135_id5)||notify.publicationRef.comment.targetType=wos||notify.publicationRef.comment.publication.id=(OPQA-4135_id2)</t>
   </si>
   <si>
     <t>1PSEARCHV4</t>
@@ -484,6 +475,24 @@
   </si>
   <si>
     <t>Verify that user can delete the comments user authored themselves and validate the comment count.</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent||notify.issuer=(SYS_USER1)||notify.issuer=(SYS_USER3)||notify.targetId=(OPQA-4135_id1)||notify.publicationRef.comment.content=(OPQA-4135_id6)||notify.publicationRef.comment.targetType=patents||notify.publicationRef.comment.publication.id=(OPQA-4135_id4)</t>
+  </si>
+  <si>
+    <t>{"queryRef":"notifyQrRef_V2","params":{"size":["20"],"byscore":"false"}}</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent||notify.issuer=(SYS_USER1)||notify.issuer=(SYS_USER3)||notify.publicationRef.comment.targetType=wos||notify.publicationRef.comment.publication.id=(OPQA-4135_id2)||notify.targetId=(OPQA-4135_id0)||notify.publicationRef.comment.content=(OPQA-4135_id5)</t>
+  </si>
+  <si>
+    <t>OPQA-236||OPQA-284||OPQA-284_1</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER2)||notify.comments.content=(OPQA-236_comments.content)||notify.document.id=(OPQA-874_hits.id)||notify.document.type=wos</t>
   </si>
 </sst>
 </file>
@@ -911,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L44"/>
+      <selection activeCell="L2" sqref="L2:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1059,7 +1068,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>36</v>
@@ -1077,506 +1086,479 @@
         <v>37</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30">
-      <c r="A6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="J6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="47.25">
+      <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="J7" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="60">
+      <c r="A9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="105">
+      <c r="A10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="45">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="7" t="s">
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" ht="45">
-      <c r="A7" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="J11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="J8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="47.25">
-      <c r="A9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="J9" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45">
-      <c r="A10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" ht="60">
-      <c r="A11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="105">
-      <c r="A12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>61</v>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" ht="45">
-      <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="J12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="105">
+      <c r="A15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
+      <c r="A16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="E16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="I13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="6" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I16" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="K16" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="D17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" ht="30">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="I17" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="30">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="105">
-      <c r="A17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I17" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="45">
-      <c r="A18" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="105">
+      <c r="A20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30">
-      <c r="A19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" ht="30">
-      <c r="A20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>110</v>
-      </c>
+      <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" ht="30">
-      <c r="A21" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60">
+      <c r="A21" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>123</v>
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="K21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="105">
-      <c r="A22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1589,7 +1571,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L8"/>
+      <selection activeCell="L2" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1676,7 +1658,7 @@
       </c>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" ht="75">
+    <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1696,16 +1678,16 @@
         <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
@@ -1728,16 +1710,16 @@
         <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="K4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45">
@@ -1760,16 +1742,16 @@
         <v>64</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>100</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
@@ -1792,16 +1774,16 @@
         <v>64</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>100</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" t="s">
         <v>127</v>
-      </c>
-      <c r="K6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
@@ -1824,16 +1806,16 @@
         <v>45</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>100</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
@@ -1856,16 +1838,16 @@
         <v>45</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>100</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1875,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2198,7 +2180,7 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
@@ -2207,7 +2189,7 @@
         <v>32</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45">
@@ -2320,7 +2302,7 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I15" t="s">
         <v>58</v>
@@ -2329,7 +2311,7 @@
         <v>32</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
@@ -2362,7 +2344,7 @@
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="45">
+    <row r="17" spans="1:12" ht="45">
       <c r="A17" t="s">
         <v>115</v>
       </c>
@@ -2392,7 +2374,7 @@
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" ht="60">
+    <row r="18" spans="1:12" ht="60">
       <c r="A18" s="3" t="s">
         <v>70</v>
       </c>
@@ -2423,7 +2405,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="105">
+    <row r="19" spans="1:12" ht="105">
       <c r="A19" s="3" t="s">
         <v>74</v>
       </c>
@@ -2453,7 +2435,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="105">
+    <row r="20" spans="1:12" ht="105">
       <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
@@ -2482,7 +2464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30">
+    <row r="21" spans="1:12" ht="30">
       <c r="A21" s="6" t="s">
         <v>120</v>
       </c>
@@ -2511,7 +2493,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="105">
+    <row r="22" spans="1:12" ht="105">
       <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
@@ -2531,11 +2513,75 @@
         <v>21</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="5" customFormat="1" ht="45">
+      <c r="A32" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32"/>
+      <c r="L32" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>